<commit_message>
Escrita de dados na planilha usando Object
</commit_message>
<xml_diff>
--- a/arquivo-planilha/src/main/java/planilhas/trabalhadores.xlsx
+++ b/arquivo-planilha/src/main/java/planilhas/trabalhadores.xlsx
@@ -108,7 +108,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>111.0</v>
+        <v>351.0</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -119,7 +119,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>222.0</v>
+        <v>521.0</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -130,7 +130,7 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>333.0</v>
+        <v>572.0</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -141,7 +141,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>444.0</v>
+        <v>701.0</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>

</xml_diff>